<commit_message>
added scraping functinoality to get all job listings of a certain class name in a url
</commit_message>
<xml_diff>
--- a/app/data/urls.xlsx
+++ b/app/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitae\OneDrive\Documents\GitHub\findify-backend\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D28393B-3AB3-49AF-A9B7-7EC912B4E042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA41ABC-C755-4715-88FE-834E66CA7868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5" yWindow="5" windowWidth="19190" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,12 +30,6 @@
     <t>Hudson River Trading</t>
   </si>
   <si>
-    <t>https://www.hudsonrivertrading.com/careers/#newjobsboard</t>
-  </si>
-  <si>
-    <t>job-title</t>
-  </si>
-  <si>
     <t>job-location-name</t>
   </si>
   <si>
@@ -61,6 +55,12 @@
   </si>
   <si>
     <t>untranslated !tw-text-xxs tw-w-fit tw-ml-auto</t>
+  </si>
+  <si>
+    <t>https://www.hudsonrivertrading.com/careers/</t>
+  </si>
+  <si>
+    <t>hrt-card-title</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -419,44 +419,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.75">
@@ -772,9 +772,6 @@
       <c r="D55" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="newjobsboard" xr:uid="{2AED68D4-A551-45AC-A853-437243CDA450}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initialized Database, setup gitignore
</commit_message>
<xml_diff>
--- a/app/data/urls.xlsx
+++ b/app/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitae\OneDrive\Documents\GitHub\findify-backend\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA41ABC-C755-4715-88FE-834E66CA7868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E0A790-FA72-468B-9CBA-004999DAFF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5" yWindow="5" windowWidth="19190" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,12 +48,6 @@
     <t>Datadog</t>
   </si>
   <si>
-    <t>https://careers.datadoghq.com/all-jobs/</t>
-  </si>
-  <si>
-    <t>job-title !tw-font-semibold untranslated</t>
-  </si>
-  <si>
     <t>untranslated !tw-text-xxs tw-w-fit tw-ml-auto</t>
   </si>
   <si>
@@ -61,6 +55,12 @@
   </si>
   <si>
     <t>hrt-card-title</t>
+  </si>
+  <si>
+    <t>job-card-title</t>
+  </si>
+  <si>
+    <t>https://careers.datadoghq.com/all-jobs/?location_Americas%5B0%5D=New%20York</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -436,10 +436,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -450,13 +450,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.75">

</xml_diff>